<commit_message>
AutoCommit_25 февраля 2024 г. 16:23:32_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -501,7 +501,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -563,7 +563,9 @@
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2">
+        <v>5</v>
+      </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -843,7 +845,9 @@
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="2">
+        <v>5</v>
+      </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_15 марта 2024 г. 10:03:52_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -501,7 +501,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
+      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -831,9 +831,15 @@
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="C24" s="2">
+        <v>5</v>
+      </c>
+      <c r="D24" s="2">
+        <v>5</v>
+      </c>
+      <c r="E24" s="2">
+        <v>5</v>
+      </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -848,8 +854,12 @@
       <c r="C25" s="2">
         <v>5</v>
       </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="D25" s="2">
+        <v>5</v>
+      </c>
+      <c r="E25" s="2">
+        <v>5</v>
+      </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_15 марта 2024 г. 10:13:44_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -501,7 +501,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -593,9 +593,13 @@
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2">
+        <v>5</v>
+      </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2">
+        <v>5</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_22 марта 2024 г. 10:08:34_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -501,7 +501,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -689,7 +689,9 @@
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2">
+        <v>5</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_22 марта 2024 г. 10:22:27_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -501,7 +501,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -833,8 +833,12 @@
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="E22" s="2">
+        <v>5</v>
+      </c>
+      <c r="F22" s="2">
+        <v>5</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_22 марта 2024 г. 10:23:09_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -501,7 +501,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -831,8 +831,12 @@
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="C22" s="2">
+        <v>5</v>
+      </c>
+      <c r="D22" s="2">
+        <v>5</v>
+      </c>
       <c r="E22" s="2">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_29 марта 2024 г. 10:06:31_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -501,7 +501,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F25" sqref="F25"/>
+      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -695,12 +695,18 @@
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="C13" s="2">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2">
+        <v>5</v>
+      </c>
       <c r="E13" s="2">
         <v>5</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2">
+        <v>5</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_29 марта 2024 г. 10:10:26_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -501,7 +501,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -585,10 +585,18 @@
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="C6" s="2">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
@@ -633,10 +641,18 @@
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="C9" s="2">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2">
+        <v>5</v>
+      </c>
+      <c r="F9" s="2">
+        <v>5</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
@@ -1016,8 +1032,12 @@
         <v>28</v>
       </c>
       <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
+      <c r="D31" s="2">
+        <v>5</v>
+      </c>
+      <c r="E31" s="2">
+        <v>5</v>
+      </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_29 марта 2024 г. 10:16:26_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -501,7 +501,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -551,7 +551,9 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2">
+        <v>5</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -627,10 +629,18 @@
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="C8" s="2">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
@@ -677,9 +687,15 @@
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="C11" s="2">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2">
+        <v>5</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_29 марта 2024 г. 11:56:50_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -501,7 +501,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -673,10 +673,18 @@
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="C10" s="2">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>5</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
@@ -835,7 +843,9 @@
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="2">
+        <v>5</v>
+      </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -849,7 +859,9 @@
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" s="2">
+        <v>5</v>
+      </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2">
         <v>5</v>
@@ -963,7 +975,9 @@
       <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="2"/>
+      <c r="C26" s="2">
+        <v>5</v>
+      </c>
       <c r="D26" s="2">
         <v>5</v>
       </c>
@@ -983,10 +997,18 @@
       <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="C27" s="2">
+        <v>5</v>
+      </c>
+      <c r="D27" s="2">
+        <v>5</v>
+      </c>
+      <c r="E27" s="2">
+        <v>5</v>
+      </c>
+      <c r="F27" s="2">
+        <v>5</v>
+      </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
@@ -1033,10 +1055,18 @@
       <c r="B30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="C30" s="2">
+        <v>5</v>
+      </c>
+      <c r="D30" s="2">
+        <v>5</v>
+      </c>
+      <c r="E30" s="2">
+        <v>5</v>
+      </c>
+      <c r="F30" s="2">
+        <v>5</v>
+      </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_5 апреля 2024 г. 10:52:59_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -501,7 +501,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -757,9 +757,15 @@
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="C14" s="2">
+        <v>5</v>
+      </c>
+      <c r="D14" s="2">
+        <v>5</v>
+      </c>
+      <c r="E14" s="2">
+        <v>5</v>
+      </c>
       <c r="F14" s="2">
         <v>5</v>
       </c>
@@ -773,8 +779,12 @@
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="C15" s="2">
+        <v>5</v>
+      </c>
+      <c r="D15" s="2">
+        <v>5</v>
+      </c>
       <c r="E15" s="2">
         <v>5</v>
       </c>
@@ -791,9 +801,15 @@
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="C16" s="2">
+        <v>5</v>
+      </c>
+      <c r="D16" s="2">
+        <v>5</v>
+      </c>
+      <c r="E16" s="2">
+        <v>5</v>
+      </c>
       <c r="F16" s="2">
         <v>5</v>
       </c>
@@ -807,9 +823,15 @@
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="C17" s="2">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2">
+        <v>5</v>
+      </c>
+      <c r="E17" s="2">
+        <v>5</v>
+      </c>
       <c r="F17" s="2">
         <v>5</v>
       </c>
@@ -846,7 +868,9 @@
       <c r="C19" s="2">
         <v>5</v>
       </c>
-      <c r="D19" s="2"/>
+      <c r="D19" s="2">
+        <v>5</v>
+      </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -879,8 +903,12 @@
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="C21" s="2">
+        <v>5</v>
+      </c>
+      <c r="D21" s="2">
+        <v>5</v>
+      </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2">
         <v>5</v>
@@ -920,7 +948,9 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="F23" s="2">
+        <v>5</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_9 апреля 2024 г. 11:40:33_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -501,7 +501,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1071,10 +1071,18 @@
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="C29" s="2">
+        <v>5</v>
+      </c>
+      <c r="D29" s="2">
+        <v>5</v>
+      </c>
+      <c r="E29" s="2">
+        <v>5</v>
+      </c>
+      <c r="F29" s="2">
+        <v>5</v>
+      </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_11 апреля 2024 г. 20:26:46_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -151,12 +151,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -186,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -196,6 +202,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -501,13 +510,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J20" sqref="J20"/>
+      <selection pane="bottomRight" activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -517,12 +526,12 @@
     <col min="3" max="8" width="5.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>29</v>
       </c>
@@ -540,7 +549,7 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -554,19 +563,25 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2">
-        <v>5</v>
-      </c>
-      <c r="F4" s="2"/>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>5</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4">
@@ -576,24 +591,27 @@
       <c r="J4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2">
-        <v>5</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="C5" s="4">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4">
+        <v>5</v>
+      </c>
+      <c r="F5" s="4">
         <v>5</v>
       </c>
       <c r="G5" s="2"/>
@@ -605,24 +623,27 @@
       <c r="J5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2">
-        <v>5</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="C6" s="4">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4">
         <v>5</v>
       </c>
       <c r="G6" s="2"/>
@@ -634,22 +655,27 @@
       <c r="J6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2">
-        <v>5</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="C7" s="4">
+        <v>5</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>5</v>
+      </c>
+      <c r="F7" s="4">
         <v>5</v>
       </c>
       <c r="G7" s="2"/>
@@ -661,24 +687,27 @@
       <c r="J7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2">
-        <v>5</v>
-      </c>
-      <c r="D8" s="2">
-        <v>5</v>
-      </c>
-      <c r="E8" s="2">
-        <v>5</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="C8" s="4">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4">
+        <v>5</v>
+      </c>
+      <c r="E8" s="4">
+        <v>5</v>
+      </c>
+      <c r="F8" s="4">
         <v>5</v>
       </c>
       <c r="G8" s="2"/>
@@ -690,24 +719,27 @@
       <c r="J8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2">
-        <v>5</v>
-      </c>
-      <c r="D9" s="2">
-        <v>5</v>
-      </c>
-      <c r="E9" s="2">
-        <v>5</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="C9" s="4">
+        <v>5</v>
+      </c>
+      <c r="D9" s="4">
+        <v>5</v>
+      </c>
+      <c r="E9" s="4">
+        <v>5</v>
+      </c>
+      <c r="F9" s="4">
         <v>5</v>
       </c>
       <c r="G9" s="2"/>
@@ -719,24 +751,27 @@
       <c r="J9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2">
-        <v>5</v>
-      </c>
-      <c r="D10" s="2">
-        <v>5</v>
-      </c>
-      <c r="E10" s="2">
-        <v>5</v>
-      </c>
-      <c r="F10" s="2">
+      <c r="C10" s="4">
+        <v>5</v>
+      </c>
+      <c r="D10" s="4">
+        <v>5</v>
+      </c>
+      <c r="E10" s="4">
+        <v>5</v>
+      </c>
+      <c r="F10" s="4">
         <v>5</v>
       </c>
       <c r="G10" s="2"/>
@@ -748,24 +783,29 @@
       <c r="J10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2">
-        <v>5</v>
-      </c>
-      <c r="D11" s="2">
-        <v>5</v>
-      </c>
-      <c r="E11" s="2">
-        <v>5</v>
-      </c>
-      <c r="F11" s="2"/>
+      <c r="C11" s="4">
+        <v>5</v>
+      </c>
+      <c r="D11" s="4">
+        <v>5</v>
+      </c>
+      <c r="E11" s="4">
+        <v>5</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11">
@@ -775,22 +815,27 @@
       <c r="J11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2">
-        <v>5</v>
-      </c>
-      <c r="E12" s="2">
-        <v>5</v>
-      </c>
-      <c r="F12" s="2">
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>5</v>
+      </c>
+      <c r="E12" s="4">
+        <v>5</v>
+      </c>
+      <c r="F12" s="4">
         <v>5</v>
       </c>
       <c r="G12" s="2"/>
@@ -802,24 +847,27 @@
       <c r="J12">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="2">
-        <v>5</v>
-      </c>
-      <c r="D13" s="2">
-        <v>5</v>
-      </c>
-      <c r="E13" s="2">
-        <v>5</v>
-      </c>
-      <c r="F13" s="2">
+      <c r="C13" s="4">
+        <v>5</v>
+      </c>
+      <c r="D13" s="4">
+        <v>5</v>
+      </c>
+      <c r="E13" s="4">
+        <v>5</v>
+      </c>
+      <c r="F13" s="4">
         <v>5</v>
       </c>
       <c r="G13" s="2"/>
@@ -831,24 +879,27 @@
       <c r="J13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="2">
-        <v>5</v>
-      </c>
-      <c r="D14" s="2">
-        <v>5</v>
-      </c>
-      <c r="E14" s="2">
-        <v>5</v>
-      </c>
-      <c r="F14" s="2">
+      <c r="C14" s="4">
+        <v>5</v>
+      </c>
+      <c r="D14" s="4">
+        <v>5</v>
+      </c>
+      <c r="E14" s="4">
+        <v>5</v>
+      </c>
+      <c r="F14" s="4">
         <v>5</v>
       </c>
       <c r="G14" s="2"/>
@@ -860,24 +911,27 @@
       <c r="J14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2">
-        <v>5</v>
-      </c>
-      <c r="D15" s="2">
-        <v>5</v>
-      </c>
-      <c r="E15" s="2">
-        <v>5</v>
-      </c>
-      <c r="F15" s="2">
+      <c r="C15" s="4">
+        <v>5</v>
+      </c>
+      <c r="D15" s="4">
+        <v>5</v>
+      </c>
+      <c r="E15" s="4">
+        <v>5</v>
+      </c>
+      <c r="F15" s="4">
         <v>5</v>
       </c>
       <c r="G15" s="2"/>
@@ -889,24 +943,27 @@
       <c r="J15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="2">
-        <v>5</v>
-      </c>
-      <c r="D16" s="2">
-        <v>5</v>
-      </c>
-      <c r="E16" s="2">
-        <v>5</v>
-      </c>
-      <c r="F16" s="2">
+      <c r="C16" s="4">
+        <v>5</v>
+      </c>
+      <c r="D16" s="4">
+        <v>5</v>
+      </c>
+      <c r="E16" s="4">
+        <v>5</v>
+      </c>
+      <c r="F16" s="4">
         <v>5</v>
       </c>
       <c r="G16" s="2"/>
@@ -918,24 +975,27 @@
       <c r="J16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="2">
-        <v>5</v>
-      </c>
-      <c r="D17" s="2">
-        <v>5</v>
-      </c>
-      <c r="E17" s="2">
-        <v>5</v>
-      </c>
-      <c r="F17" s="2">
+      <c r="C17" s="4">
+        <v>5</v>
+      </c>
+      <c r="D17" s="4">
+        <v>5</v>
+      </c>
+      <c r="E17" s="4">
+        <v>5</v>
+      </c>
+      <c r="F17" s="4">
         <v>5</v>
       </c>
       <c r="G17" s="2"/>
@@ -947,22 +1007,27 @@
       <c r="J17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2">
-        <v>5</v>
-      </c>
-      <c r="E18" s="2">
-        <v>5</v>
-      </c>
-      <c r="F18" s="2">
+      <c r="C18" s="4">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
+        <v>5</v>
+      </c>
+      <c r="E18" s="4">
+        <v>5</v>
+      </c>
+      <c r="F18" s="4">
         <v>5</v>
       </c>
       <c r="G18" s="2"/>
@@ -974,22 +1039,29 @@
       <c r="J18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="2">
-        <v>5</v>
-      </c>
-      <c r="D19" s="2">
-        <v>5</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="C19" s="4">
+        <v>5</v>
+      </c>
+      <c r="D19" s="4">
+        <v>5</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19">
@@ -999,22 +1071,27 @@
       <c r="J19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="2">
-        <v>5</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2">
-        <v>5</v>
-      </c>
-      <c r="F20" s="2">
+      <c r="C20" s="4">
+        <v>5</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4">
+        <v>5</v>
+      </c>
+      <c r="F20" s="4">
         <v>5</v>
       </c>
       <c r="G20" s="2"/>
@@ -1026,22 +1103,27 @@
       <c r="J20">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="2">
-        <v>5</v>
-      </c>
-      <c r="D21" s="2">
-        <v>5</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2">
+      <c r="C21" s="4">
+        <v>5</v>
+      </c>
+      <c r="D21" s="4">
+        <v>5</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
         <v>5</v>
       </c>
       <c r="G21" s="2"/>
@@ -1053,24 +1135,27 @@
       <c r="J21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="2">
-        <v>5</v>
-      </c>
-      <c r="D22" s="2">
-        <v>5</v>
-      </c>
-      <c r="E22" s="2">
-        <v>5</v>
-      </c>
-      <c r="F22" s="2">
+      <c r="C22" s="4">
+        <v>5</v>
+      </c>
+      <c r="D22" s="4">
+        <v>5</v>
+      </c>
+      <c r="E22" s="4">
+        <v>5</v>
+      </c>
+      <c r="F22" s="4">
         <v>5</v>
       </c>
       <c r="G22" s="2"/>
@@ -1082,24 +1167,27 @@
       <c r="J22">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="2">
-        <v>5</v>
-      </c>
-      <c r="D23" s="2">
-        <v>5</v>
-      </c>
-      <c r="E23" s="2">
-        <v>5</v>
-      </c>
-      <c r="F23" s="2">
+      <c r="C23" s="4">
+        <v>5</v>
+      </c>
+      <c r="D23" s="4">
+        <v>5</v>
+      </c>
+      <c r="E23" s="4">
+        <v>5</v>
+      </c>
+      <c r="F23" s="4">
         <v>5</v>
       </c>
       <c r="G23" s="2"/>
@@ -1111,24 +1199,27 @@
       <c r="J23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="2">
-        <v>5</v>
-      </c>
-      <c r="D24" s="2">
-        <v>5</v>
-      </c>
-      <c r="E24" s="2">
-        <v>5</v>
-      </c>
-      <c r="F24" s="2">
+      <c r="C24" s="4">
+        <v>5</v>
+      </c>
+      <c r="D24" s="4">
+        <v>5</v>
+      </c>
+      <c r="E24" s="4">
+        <v>5</v>
+      </c>
+      <c r="F24" s="4">
         <v>5</v>
       </c>
       <c r="G24" s="2"/>
@@ -1140,24 +1231,27 @@
       <c r="J24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="2">
-        <v>5</v>
-      </c>
-      <c r="D25" s="2">
-        <v>5</v>
-      </c>
-      <c r="E25" s="2">
-        <v>5</v>
-      </c>
-      <c r="F25" s="2">
+      <c r="C25" s="4">
+        <v>5</v>
+      </c>
+      <c r="D25" s="4">
+        <v>5</v>
+      </c>
+      <c r="E25" s="4">
+        <v>5</v>
+      </c>
+      <c r="F25" s="4">
         <v>5</v>
       </c>
       <c r="G25" s="2"/>
@@ -1169,24 +1263,27 @@
       <c r="J25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="2">
-        <v>5</v>
-      </c>
-      <c r="D26" s="2">
-        <v>5</v>
-      </c>
-      <c r="E26" s="2">
-        <v>5</v>
-      </c>
-      <c r="F26" s="2">
+      <c r="C26" s="4">
+        <v>5</v>
+      </c>
+      <c r="D26" s="4">
+        <v>5</v>
+      </c>
+      <c r="E26" s="4">
+        <v>5</v>
+      </c>
+      <c r="F26" s="4">
         <v>5</v>
       </c>
       <c r="G26" s="2"/>
@@ -1198,24 +1295,27 @@
       <c r="J26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="2">
-        <v>5</v>
-      </c>
-      <c r="D27" s="2">
-        <v>5</v>
-      </c>
-      <c r="E27" s="2">
-        <v>5</v>
-      </c>
-      <c r="F27" s="2">
+      <c r="C27" s="4">
+        <v>5</v>
+      </c>
+      <c r="D27" s="4">
+        <v>5</v>
+      </c>
+      <c r="E27" s="4">
+        <v>5</v>
+      </c>
+      <c r="F27" s="4">
         <v>5</v>
       </c>
       <c r="G27" s="2"/>
@@ -1227,24 +1327,27 @@
       <c r="J27">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="2">
-        <v>5</v>
-      </c>
-      <c r="D28" s="2">
-        <v>5</v>
-      </c>
-      <c r="E28" s="2">
-        <v>5</v>
-      </c>
-      <c r="F28" s="2">
+      <c r="C28" s="4">
+        <v>5</v>
+      </c>
+      <c r="D28" s="4">
+        <v>5</v>
+      </c>
+      <c r="E28" s="4">
+        <v>5</v>
+      </c>
+      <c r="F28" s="4">
         <v>5</v>
       </c>
       <c r="G28" s="2"/>
@@ -1256,24 +1359,27 @@
       <c r="J28">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="2">
-        <v>5</v>
-      </c>
-      <c r="D29" s="2">
-        <v>5</v>
-      </c>
-      <c r="E29" s="2">
-        <v>5</v>
-      </c>
-      <c r="F29" s="2">
+      <c r="C29" s="4">
+        <v>5</v>
+      </c>
+      <c r="D29" s="4">
+        <v>5</v>
+      </c>
+      <c r="E29" s="4">
+        <v>5</v>
+      </c>
+      <c r="F29" s="4">
         <v>5</v>
       </c>
       <c r="G29" s="2"/>
@@ -1285,24 +1391,27 @@
       <c r="J29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="2">
-        <v>5</v>
-      </c>
-      <c r="D30" s="2">
-        <v>5</v>
-      </c>
-      <c r="E30" s="2">
-        <v>5</v>
-      </c>
-      <c r="F30" s="2">
+      <c r="C30" s="4">
+        <v>5</v>
+      </c>
+      <c r="D30" s="4">
+        <v>5</v>
+      </c>
+      <c r="E30" s="4">
+        <v>5</v>
+      </c>
+      <c r="F30" s="4">
         <v>5</v>
       </c>
       <c r="G30" s="2"/>
@@ -1314,22 +1423,29 @@
       <c r="J30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="K30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2">
-        <v>5</v>
-      </c>
-      <c r="E31" s="2">
-        <v>5</v>
-      </c>
-      <c r="F31" s="2"/>
+      <c r="C31" s="4">
+        <v>0</v>
+      </c>
+      <c r="D31" s="4">
+        <v>5</v>
+      </c>
+      <c r="E31" s="4">
+        <v>5</v>
+      </c>
+      <c r="F31" s="4">
+        <v>0</v>
+      </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31">
@@ -1339,8 +1455,11 @@
       <c r="J31">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>

</xml_diff>

<commit_message>
AutoCommit_11 апреля 2024 г. 22:15:47_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -513,10 +513,10 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K32" sqref="K32"/>
+      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1019,7 +1019,7 @@
         <v>15</v>
       </c>
       <c r="C18" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D18" s="4">
         <v>5</v>
@@ -1034,7 +1034,7 @@
       <c r="H18" s="2"/>
       <c r="I18">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J18">
         <v>4</v>

</xml_diff>

<commit_message>
AutoCommit_12 апреля 2024 г. 10:07:49_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -133,7 +133,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -150,8 +150,15 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +168,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -192,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -204,6 +217,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -513,10 +532,10 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -669,8 +688,8 @@
       <c r="C7" s="4">
         <v>5</v>
       </c>
-      <c r="D7" s="4">
-        <v>0</v>
+      <c r="D7" s="6">
+        <v>5</v>
       </c>
       <c r="E7" s="4">
         <v>5</v>
@@ -682,7 +701,7 @@
       <c r="H7" s="2"/>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J7">
         <v>4</v>
@@ -826,8 +845,8 @@
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="4">
-        <v>0</v>
+      <c r="C12" s="5">
+        <v>5</v>
       </c>
       <c r="D12" s="4">
         <v>5</v>
@@ -842,7 +861,7 @@
       <c r="H12" s="2"/>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J12">
         <v>4</v>
@@ -1482,5 +1501,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AutoCommit_12 апреля 2024 г. 10:12:30_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -535,7 +535,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -589,23 +589,23 @@
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0</v>
+      <c r="C4" s="6">
+        <v>5</v>
+      </c>
+      <c r="D4" s="6">
+        <v>5</v>
       </c>
       <c r="E4" s="4">
         <v>5</v>
       </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2"/>
+      <c r="F4" s="6">
+        <v>5</v>
+      </c>
+      <c r="G4" s="6"/>
       <c r="H4" s="2"/>
       <c r="I4">
         <f>SUM(C4:H4)</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -1453,8 +1453,8 @@
       <c r="B31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="4">
-        <v>0</v>
+      <c r="C31" s="6">
+        <v>5</v>
       </c>
       <c r="D31" s="4">
         <v>5</v>
@@ -1462,14 +1462,14 @@
       <c r="E31" s="4">
         <v>5</v>
       </c>
-      <c r="F31" s="4">
-        <v>0</v>
+      <c r="F31" s="6">
+        <v>5</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J31">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_12 апреля 2024 г. 11:40:23_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -535,7 +535,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -822,14 +822,14 @@
       <c r="E11" s="4">
         <v>5</v>
       </c>
-      <c r="F11" s="4">
-        <v>0</v>
+      <c r="F11" s="5">
+        <v>5</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J11">
         <v>4</v>

</xml_diff>

<commit_message>
AutoCommit_31 мая 2024 г. 11:01:01_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -541,10 +541,10 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1384,11 +1384,13 @@
       <c r="F28" s="4">
         <v>5</v>
       </c>
-      <c r="G28" s="2"/>
+      <c r="G28" s="2">
+        <v>5</v>
+      </c>
       <c r="H28" s="2"/>
       <c r="I28">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J28">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_10 июня 2024 г. 11:51:24_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>2ИСИП-622: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -123,10 +123,7 @@
     <t>ДЗ_5</t>
   </si>
   <si>
-    <t>сумм</t>
-  </si>
-  <si>
-    <t>тк</t>
+    <t>лаб1</t>
   </si>
 </sst>
 </file>
@@ -184,7 +181,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -207,11 +204,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -232,6 +249,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -538,13 +561,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G28" sqref="G28"/>
+      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -554,12 +577,12 @@
     <col min="3" max="8" width="5.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>29</v>
       </c>
@@ -578,22 +601,22 @@
       <c r="H2" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>7</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -614,18 +637,8 @@
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="2"/>
-      <c r="I4">
-        <f>SUM(C4:H4)</f>
-        <v>20</v>
-      </c>
-      <c r="J4">
-        <v>3</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -646,18 +659,8 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5">
-        <f t="shared" ref="I5:I31" si="0">SUM(C5:H5)</f>
-        <v>20</v>
-      </c>
-      <c r="J5">
-        <v>5</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -678,18 +681,8 @@
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J6">
-        <v>5</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -710,18 +703,8 @@
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J7">
-        <v>4</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -740,20 +723,17 @@
       <c r="F8" s="4">
         <v>5</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J8">
-        <v>5</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="G8" s="2">
+        <v>5</v>
+      </c>
+      <c r="H8" s="2">
+        <v>5</v>
+      </c>
+      <c r="I8" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -774,18 +754,8 @@
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J9">
-        <v>5</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -806,18 +776,8 @@
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J10">
-        <v>5</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -836,20 +796,14 @@
       <c r="F11" s="5">
         <v>5</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J11">
-        <v>4</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="G11" s="2">
+        <v>5</v>
+      </c>
+      <c r="H11" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -870,18 +824,8 @@
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J12">
-        <v>4</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -902,18 +846,8 @@
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J13">
-        <v>5</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -934,18 +868,8 @@
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J14">
-        <v>5</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -966,18 +890,8 @@
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J15">
-        <v>5</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -998,18 +912,8 @@
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="I16">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J16">
-        <v>5</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -1030,18 +934,8 @@
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J17">
-        <v>5</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1062,18 +956,8 @@
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J18">
-        <v>4</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1094,18 +978,8 @@
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="I19">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="J19">
-        <v>3</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1126,18 +1000,8 @@
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-      <c r="I20">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J20">
-        <v>4</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -1158,18 +1022,8 @@
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-      <c r="I21">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="J21">
-        <v>4</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1194,18 +1048,8 @@
       <c r="H22" s="2">
         <v>5</v>
       </c>
-      <c r="I22">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="J22">
-        <v>5</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -1226,18 +1070,8 @@
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
-      <c r="I23">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J23">
-        <v>5</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -1258,18 +1092,8 @@
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-      <c r="I24">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J24">
-        <v>5</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -1290,18 +1114,8 @@
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-      <c r="I25">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J25">
-        <v>5</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -1322,18 +1136,8 @@
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
-      <c r="I26">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J26">
-        <v>5</v>
-      </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -1354,18 +1158,8 @@
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
-      <c r="I27">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J27">
-        <v>5</v>
-      </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -1387,19 +1181,14 @@
       <c r="G28" s="2">
         <v>5</v>
       </c>
-      <c r="H28" s="2"/>
-      <c r="I28">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="J28">
-        <v>5</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="H28" s="2">
+        <v>5</v>
+      </c>
+      <c r="I28" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -1420,18 +1209,8 @@
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
-      <c r="I29">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J29">
-        <v>5</v>
-      </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -1452,18 +1231,8 @@
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
-      <c r="I30">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J30">
-        <v>5</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:9" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -1484,18 +1253,8 @@
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
-      <c r="I31">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="J31">
-        <v>3</v>
-      </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -1505,7 +1264,7 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="I4:I31">
+  <conditionalFormatting sqref="I4:I27 I29:I31">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
AutoCommit_10 июня 2024 г. 14:11:03_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -567,7 +567,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomRight" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -803,7 +803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -825,7 +825,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -844,10 +844,17 @@
       <c r="F13" s="4">
         <v>5</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+      <c r="G13" s="2">
+        <v>5</v>
+      </c>
+      <c r="H13" s="2">
+        <v>5</v>
+      </c>
+      <c r="I13" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -891,7 +898,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:10" ht="13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -913,7 +920,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -932,10 +939,17 @@
       <c r="F17" s="4">
         <v>5</v>
       </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="G17" s="2">
+        <v>5</v>
+      </c>
+      <c r="H17" s="2">
+        <v>5</v>
+      </c>
+      <c r="I17" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1264,7 +1278,7 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="I4:I27 I29:I31">
+  <conditionalFormatting sqref="I4:I12 I29:I31 I14:I16 I18:I27">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
AutoCommit_10 июня 2024 г. 14:11:44_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -567,7 +567,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I17" sqref="I17"/>
+      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -800,6 +800,9 @@
         <v>5</v>
       </c>
       <c r="H11" s="2">
+        <v>5</v>
+      </c>
+      <c r="I11">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AutoCommit_11 июня 2024 г. 10:45:23_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -228,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -255,6 +255,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -564,10 +567,10 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomRight" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -923,7 +926,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -951,8 +954,11 @@
       <c r="I17" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J17" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -974,7 +980,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -996,7 +1002,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1018,7 +1024,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -1040,7 +1046,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1066,7 +1072,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -1088,7 +1094,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -1110,7 +1116,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -1132,7 +1138,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -1154,7 +1160,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -1176,7 +1182,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -1205,7 +1211,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -1227,7 +1233,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -1249,7 +1255,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -1271,7 +1277,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>

</xml_diff>

<commit_message>
AutoCommit_11 июня 2024 г. 10:47:35_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -566,11 +566,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J19" sqref="J19"/>
+      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -704,8 +704,18 @@
       <c r="F7" s="4">
         <v>5</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="G7" s="2">
+        <v>5</v>
+      </c>
+      <c r="H7" s="2">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">

</xml_diff>

<commit_message>
AutoCommit_13 июня 2024 г. 8:52:33_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -576,7 +576,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomRight" activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1090,8 +1090,18 @@
       <c r="F20" s="4">
         <v>5</v>
       </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="G20" s="2">
+        <v>5</v>
+      </c>
+      <c r="H20" s="2">
+        <v>5</v>
+      </c>
+      <c r="I20">
+        <v>5</v>
+      </c>
+      <c r="J20">
+        <v>5</v>
+      </c>
     </row>
     <row r="21" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">

</xml_diff>

<commit_message>
AutoCommit_14 июня 2024 г. 10:55:47_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -576,7 +576,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
+      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1336,8 +1336,15 @@
       <c r="F27" s="4">
         <v>5</v>
       </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
+      <c r="G27" s="2">
+        <v>5</v>
+      </c>
+      <c r="H27" s="2">
+        <v>5</v>
+      </c>
+      <c r="I27" s="11">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">

</xml_diff>

<commit_message>
AutoCommit_14 июня 2024 г. 11:25:22_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -573,10 +573,10 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
+      <selection pane="bottomRight" activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1426,8 +1426,15 @@
       <c r="F30" s="4">
         <v>5</v>
       </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
+      <c r="G30" s="2">
+        <v>5</v>
+      </c>
+      <c r="H30" s="2">
+        <v>5</v>
+      </c>
+      <c r="I30" s="11">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">

</xml_diff>

<commit_message>
AutoCommit_15 июня 2024 г. 23:22:15_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -228,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -267,6 +267,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -621,12 +624,30 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="13" x14ac:dyDescent="0.25">
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="14">
+        <v>1</v>
+      </c>
+      <c r="J3" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -717,7 +738,9 @@
       <c r="H6" s="2">
         <v>5</v>
       </c>
-      <c r="I6" s="9"/>
+      <c r="I6" s="9">
+        <v>2</v>
+      </c>
       <c r="J6" s="9">
         <v>5</v>
       </c>
@@ -837,8 +860,18 @@
       <c r="F10" s="4">
         <v>5</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="G10" s="2">
+        <v>2</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2</v>
+      </c>
+      <c r="I10" s="11">
+        <v>2</v>
+      </c>
+      <c r="J10" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -1028,6 +1061,9 @@
       <c r="I16" s="11">
         <v>5</v>
       </c>
+      <c r="J16" s="11">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
@@ -1107,13 +1143,23 @@
         <v>5</v>
       </c>
       <c r="E19" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F19" s="4">
-        <v>0</v>
-      </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="G19" s="2">
+        <v>2</v>
+      </c>
+      <c r="H19" s="2">
+        <v>2</v>
+      </c>
+      <c r="I19" s="11">
+        <v>2</v>
+      </c>
+      <c r="J19" s="11">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
@@ -1371,6 +1417,9 @@
       <c r="I27" s="11">
         <v>5</v>
       </c>
+      <c r="J27" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="1:11" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
@@ -1429,6 +1478,9 @@
       <c r="H29" s="2">
         <v>5</v>
       </c>
+      <c r="I29" s="11">
+        <v>2</v>
+      </c>
       <c r="J29" s="12">
         <v>5</v>
       </c>
@@ -1460,6 +1512,9 @@
       </c>
       <c r="I30" s="11">
         <v>5</v>
+      </c>
+      <c r="J30" s="12">
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="13" x14ac:dyDescent="0.25">
@@ -1504,7 +1559,7 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="I4:I12 I29:I31 I14:I16 I18:I27 J12 J21:K21 J18 K24 J8:J9 J29 J22:J26 J4:J6">
+  <conditionalFormatting sqref="I4:I12 I29:I31 I14:I16 I18:I27 J12 J21:K21 K24 J4:J6 J18:J19 J8:J10 J16 J22:J27 J29:J30">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
AutoCommit_16 июня 2024 г. 12:58:56_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-622_ТерВер.xlsx
+++ b/_2ИСИП-622_ТерВер.xlsx
@@ -555,10 +555,10 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M31" sqref="M31"/>
+      <selection pane="bottomRight" activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>